<commit_message>
Created csv version of Elephas PA
</commit_message>
<xml_diff>
--- a/data/about_data_points.xlsx
+++ b/data/about_data_points.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t-r-espr/Documents/class/Master Thesis/sdm-asian-elephants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64878889-51AC-204F-A225-AFD0B3B744E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD72737F-DC3E-DF44-9797-8E70E31BDBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16940" activeTab="2" xr2:uid="{B70DE5DD-E91B-B943-AA99-96FD8C7C0097}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16940" activeTab="1" xr2:uid="{B70DE5DD-E91B-B943-AA99-96FD8C7C0097}"/>
   </bookViews>
   <sheets>
     <sheet name="climate_vars" sheetId="1" r:id="rId1"/>
-    <sheet name="elephas_presence" sheetId="2" r:id="rId2"/>
-    <sheet name="grid_centers" sheetId="3" r:id="rId3"/>
+    <sheet name="future_climate" sheetId="4" r:id="rId2"/>
+    <sheet name="elephas_presence" sheetId="2" r:id="rId3"/>
+    <sheet name="grid_centers" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
   <si>
     <t>HID</t>
   </si>
@@ -314,24 +315,183 @@
   <si>
     <t>This ties the climatic variables to the geodesic grid.</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WC30AS_V14: The 30 arc seconds climate surface data from Hijimans et al. 2005, available as the WorldClim database. This SDM is based on version 1.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CMIP5: The climate model being used</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CCSM4: Another climate model, Community Climate System Model 4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RCP85: RCP8.5 - A global warming scenario that assumes nobody cooperated in preventing climate change</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2070: This is a prediction for 2070</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BIO01_Mean</t>
+  </si>
+  <si>
+    <t>BIO02_Mean</t>
+  </si>
+  <si>
+    <t>BIO03_Mean</t>
+  </si>
+  <si>
+    <t>BIO04_Mean</t>
+  </si>
+  <si>
+    <t>BIO05_Mean</t>
+  </si>
+  <si>
+    <t>BIO06_Mean</t>
+  </si>
+  <si>
+    <t>BIO07_Mean</t>
+  </si>
+  <si>
+    <t>BIO08_Mean</t>
+  </si>
+  <si>
+    <t>BIO09_Mean</t>
+  </si>
+  <si>
+    <t>BIO10_Mean</t>
+  </si>
+  <si>
+    <t>BIO11_Mean</t>
+  </si>
+  <si>
+    <t>BIO12_Mean</t>
+  </si>
+  <si>
+    <t>BIO13_Mean</t>
+  </si>
+  <si>
+    <t>BIO14_Mean</t>
+  </si>
+  <si>
+    <t>BIO15_Mean</t>
+  </si>
+  <si>
+    <t>BIO16_Mean</t>
+  </si>
+  <si>
+    <t>BIO17_Mean</t>
+  </si>
+  <si>
+    <t>BIO18_Mean</t>
+  </si>
+  <si>
+    <t>BIO19_Mean</t>
+  </si>
+  <si>
+    <t>Annual Mean Temperature</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mean Diurnal Range (Mean of monthly (max temp - min temp))</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Isothermality (BIO2/BIO7) (×100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Temperature Seasonality (standard deviation ×100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Max Temperature of Warmest Month</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Min Temperature of Coldest Month</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Temperature Annual Range (BIO5-BIO6)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mean Temperature of Wettest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mean Temperature of Driest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mean Temperature of Warmest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mean Temperature of Coldest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Annual Precipitation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Wettest Month</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Driest Month</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation Seasonality (Coefficient of Variation)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Wettest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Driest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Warmest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Precipitation of Coldest Quarter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://www.worldclim.org/data/bioclim.html</t>
+  </si>
+  <si>
+    <t>ISEA3H09_WC30AS_V14_CMIP5_CCSM4_RCP85_2070_BIO.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -339,7 +499,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -347,7 +507,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -387,7 +547,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -403,7 +563,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -702,50 +862,50 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A18:A19"/>
+      <selection activeCell="A10" sqref="A10:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -753,7 +913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -761,7 +921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -769,7 +929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -777,7 +937,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -785,7 +945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -793,7 +953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -801,7 +961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -809,7 +969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -817,7 +977,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -825,7 +985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -833,7 +993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -841,7 +1001,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -849,7 +1009,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -857,7 +1017,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -865,7 +1025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -873,7 +1033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -881,7 +1041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -889,7 +1049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -897,7 +1057,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -905,7 +1065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -913,7 +1073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -921,7 +1081,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -929,7 +1089,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -937,7 +1097,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -945,7 +1105,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -953,7 +1113,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -961,7 +1121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -976,6 +1136,220 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2966255D-2337-9447-A73D-B6D0073FE866}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46B641-FEA2-D147-9141-56B2AB9F2AB9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -983,24 +1357,24 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1008,7 +1382,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1022,32 +1396,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90893035-47DA-C24A-9518-463A236A3769}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1055,7 +1429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1063,7 +1437,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Updated info about the files
</commit_message>
<xml_diff>
--- a/data/about_data_points.xlsx
+++ b/data/about_data_points.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t-r-espr/Documents/class/Master Thesis/sdm-asian-elephants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD72737F-DC3E-DF44-9797-8E70E31BDBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3A5178-3C1E-7D47-9AB2-FE0B55486A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16940" activeTab="1" xr2:uid="{B70DE5DD-E91B-B943-AA99-96FD8C7C0097}"/>
   </bookViews>
   <sheets>
-    <sheet name="climate_vars" sheetId="1" r:id="rId1"/>
-    <sheet name="future_climate" sheetId="4" r:id="rId2"/>
+    <sheet name="etccdi_climate" sheetId="1" r:id="rId1"/>
+    <sheet name="wc30as_climate" sheetId="4" r:id="rId2"/>
     <sheet name="elephas_presence" sheetId="2" r:id="rId3"/>
     <sheet name="grid_centers" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
   <si>
     <t>HID</t>
   </si>
@@ -120,37 +120,14 @@
     <t>WSDI_IDW1N10</t>
   </si>
   <si>
-    <t>The climate variables per hexagonal grid in ISEA3H09_CCSM4_Y1950_Y2000_ETCCDI_IDW1N10.txt</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>CCSM4: The name of the simulated climate model. Community Climate System Model 4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Y1950_Y2000: The year the model covers</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ETCCDI: The name of the climate indices used as features. Named after the organization that invented them</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ISEA3H09: The geodesic grid system. Icosahedron Snyder Equal Area Aperture 3 Hexagonal grid system. 09 probably stands for the granularity, if I remenber right it was the most granular</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IDW1N10: The interpolation method used on the data. Inverse Distance Weighted interpolation with 10 neighbors</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>The hexagon ID</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>http://etccdi.pacificclimate.org/list_27_indices.shtml</t>
-  </si>
-  <si>
     <t>Maximum length of dry spell, maximum number of consecutive days with daily precipitation &lt; 1mm</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -321,22 +298,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CMIP5: The climate model being used</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CCSM4: Another climate model, Community Climate System Model 4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>RCP85: RCP8.5 - A global warming scenario that assumes nobody cooperated in preventing climate change</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2070: This is a prediction for 2070</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BIO01_Mean</t>
   </si>
   <si>
@@ -474,6 +439,39 @@
   </si>
   <si>
     <t>ISEA3H09_WC30AS_V14_CMIP5_CCSM4_RCP85_2070_BIO.txt</t>
+  </si>
+  <si>
+    <t>ISEA3H09: The geodesic grid system. Icosahedron Snyder Equal Area Aperture 3 Hexagonal grid system. 09 is the resolution. Resolution +1 splits the icosahedron planes in 3rds. 09 means approx 50km in between centroids.</t>
+  </si>
+  <si>
+    <t>IDW1N10: The interpolation method used on the data. Inverse Distance Weighted interpolation. The grids of CCSM4 was finer than ISEA3H09, so mapped 10 NN CCSM grids to one hexagon centroid</t>
+  </si>
+  <si>
+    <t>One of the climate variable files.</t>
+  </si>
+  <si>
+    <t>Past: ISEA3H09_CCSM4_Y1950_Y2000_ETCCDI_IDW1N10.txt</t>
+  </si>
+  <si>
+    <t>ETCCDI: The name of the climate indices used as features. http://etccdi.pacificclimate.org/list_27_indices.shtml</t>
+  </si>
+  <si>
+    <t>Y1950_Y2000: The year the variables for the past covers</t>
+  </si>
+  <si>
+    <t>CMIP5: An ensemble of climate models. CCSM4 is (presumably) one of them</t>
+  </si>
+  <si>
+    <t>Values -1000 means no data. Either land out of scope or the ocean</t>
+  </si>
+  <si>
+    <t>2070: This is a prediction for 2070. 2070 was the most distant features available in the dataset</t>
+  </si>
+  <si>
+    <t>"_Mean" indicates that it is a mean of the monthly or annual data from 2061-2080 (in the future data's case)</t>
+  </si>
+  <si>
+    <t>CCSM4: The climate model combined with WC30AS to predict future data. Example for estimating 2070 temperature from 2000 data: CCSM was used to predict thee difference between the temperature of 2000 and 2070, and the difference was added to the actual observed (or interpolated) temperature for 2000 in WorldClim</t>
   </si>
 </sst>
 </file>
@@ -859,11 +857,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E8BDA-E0F6-234B-9054-449E08191B30}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -872,261 +868,264 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
+      <c r="A2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>26</v>
       </c>
-      <c r="B36" t="s">
-        <v>62</v>
+      <c r="B37" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1137,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2966255D-2337-9447-A73D-B6D0073FE866}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,197 +1149,212 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1361,33 +1375,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1408,41 +1422,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished exploring ETCCDI train area variables
Need to wait for additional data for test area.
</commit_message>
<xml_diff>
--- a/data/about_data_points.xlsx
+++ b/data/about_data_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t-r-espr/Documents/class/Master Thesis/sdm-asian-elephants/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F38FC5-E5FD-3646-898D-4B591D4FD3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1DA880-FA86-054B-A3D7-036EECF5F7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28300" windowHeight="16940" xr2:uid="{B70DE5DD-E91B-B943-AA99-96FD8C7C0097}"/>
   </bookViews>
@@ -204,10 +204,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Monthly minimum value of daily maximum temperature</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Number of tropical nights: Annual count of days when daily min temperature &gt; 20 degrees C</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -468,6 +464,9 @@
   </si>
   <si>
     <t>TXX_IDW1N10</t>
+  </si>
+  <si>
+    <t>Monthly maximum value of daily minimum temperature</t>
   </si>
 </sst>
 </file>
@@ -855,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E8BDA-E0F6-234B-9054-449E08191B30}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,12 +865,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -879,7 +878,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -889,17 +888,17 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -923,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -963,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1075,7 +1074,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1083,7 +1082,7 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1099,7 +1098,7 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1107,15 +1106,15 @@
         <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1123,7 +1122,7 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1147,42 +1146,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1190,169 +1189,169 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1373,33 +1372,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1420,22 +1419,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -1443,18 +1442,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>